<commit_message>
worked on pandas data filters and summary for final prediction model
</commit_message>
<xml_diff>
--- a/manual_identification_power_surges_causing_anomaly.xlsx
+++ b/manual_identification_power_surges_causing_anomaly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Machine_Learning_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D61D854-C0C8-4D4F-B534-85578DB9C281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45C51C6-7B05-47D2-915D-927A3281F9C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{62435CC0-C078-44E7-9647-4921B47046FB}"/>
   </bookViews>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F9ED783-BDD1-4522-8DF0-8DF064ABCB60}">
   <dimension ref="A1:C452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A390" workbookViewId="0">
-      <selection activeCell="C203" sqref="C203"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="G170" sqref="G170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2125,14 +2125,14 @@
         <v>1.8230000000000004</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144">
+    <row r="144" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
         <v>8.859</v>
       </c>
-      <c r="B144">
+      <c r="B144" s="1">
         <v>14.16</v>
       </c>
-      <c r="C144">
+      <c r="C144" s="1">
         <f t="shared" si="2"/>
         <v>3.4000000000000004</v>
       </c>
@@ -2281,14 +2281,14 @@
         <v>-8.7700000000000014</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157">
+    <row r="157" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
         <v>9.86</v>
       </c>
-      <c r="B157">
+      <c r="B157" s="1">
         <v>14.845000000000001</v>
       </c>
-      <c r="C157">
+      <c r="C157" s="1">
         <f t="shared" si="2"/>
         <v>-0.54899999999999949</v>
       </c>
@@ -2353,14 +2353,14 @@
         <v>-3.2149999999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163">
+    <row r="163" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
         <v>10.085000000000001</v>
       </c>
-      <c r="B163">
+      <c r="B163" s="1">
         <v>20.709</v>
       </c>
-      <c r="C163">
+      <c r="C163" s="1">
         <f t="shared" si="2"/>
         <v>4.57</v>
       </c>

</xml_diff>